<commit_message>
Commit with no changes added
</commit_message>
<xml_diff>
--- a/TestData/RegistrationTestData_Valid.xlsx
+++ b/TestData/RegistrationTestData_Valid.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>${firstName}</t>
   </si>
@@ -88,12 +88,31 @@
   </si>
   <si>
     <t>Cairo</t>
+  </si>
+  <si>
+    <t>${password}</t>
+  </si>
+  <si>
+    <t>${confirmPassword}</t>
+  </si>
+  <si>
+    <t>samer654$%</t>
+  </si>
+  <si>
+    <t>diaa123@$</t>
+  </si>
+  <si>
+    <t>omarmohamed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="169" formatCode="00000000000"/>
+    <numFmt numFmtId="170" formatCode="0000000000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,11 +173,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,12 +493,14 @@
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -499,8 +522,14 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -510,7 +539,7 @@
       <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>1098823123</v>
       </c>
       <c r="E2" t="s">
@@ -522,8 +551,14 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -533,7 +568,7 @@
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>1082637288</v>
       </c>
       <c r="E3" t="s">
@@ -545,8 +580,14 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -556,6 +597,9 @@
       <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D4" s="4">
+        <v>1092123112</v>
+      </c>
       <c r="E4" t="s">
         <v>21</v>
       </c>
@@ -564,6 +608,12 @@
       </c>
       <c r="G4" t="s">
         <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -571,9 +621,11 @@
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
     <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="H2" r:id="rId4" display="diaa123@"/>
+    <hyperlink ref="I2" r:id="rId5" display="diaa123@"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>